<commit_message>
feat: Add improved milestone timeline with visual progress
- New MilestoneTimeline component with visual timeline track
- Shows warehouse and showroom timelines with milestone nodes
- Support for paused projects with reason display
- Progress indicators on individual milestones
- Expandable/collapsible cards for each project
- Color-coded status: complete, in-progress, upcoming, overdue
- Quick stats: target date, days remaining, milestone count
- Next milestone highlight with notes
- Configurable via Excel Settings sheet (Showroom Paused, Warehouse Paused)
</commit_message>
<xml_diff>
--- a/public/data/HOC_Investor_Dashboard_Template.xlsx
+++ b/public/data/HOC_Investor_Dashboard_Template.xlsx
@@ -1551,7 +1551,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1596,106 +1596,128 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Warehouse Location</v>
+        <v>Showroom Paused</v>
       </c>
       <c r="B4" t="str">
-        <v>UK Warehouse</v>
+        <v>Yes</v>
       </c>
       <c r="C4" t="str">
-        <v>Display name</v>
+        <v>Project currently on hold pending strategic review</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Warehouse Target Date</v>
+        <v>Warehouse Location</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-15</v>
+        <v>UK Warehouse</v>
       </c>
       <c r="C5" t="str">
-        <v>Target completion</v>
+        <v>Display name</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Gross Margin Target</v>
-      </c>
-      <c r="B6">
-        <v>45</v>
+        <v>Warehouse Target Date</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2026-01-15</v>
       </c>
       <c r="C6" t="str">
-        <v>Percentage</v>
+        <v>Target completion</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>B2B Split</v>
-      </c>
-      <c r="B7">
-        <v>60</v>
+        <v>Warehouse Paused</v>
+      </c>
+      <c r="B7" t="str">
+        <v>No</v>
       </c>
       <c r="C7" t="str">
-        <v>Percentage of revenue</v>
+        <v/>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>B2C Split</v>
+        <v>Gross Margin Target</v>
       </c>
       <c r="B8">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C8" t="str">
-        <v>Percentage of revenue</v>
+        <v>Percentage</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Staff Required</v>
+        <v>B2B Split</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="C9" t="str">
-        <v>Total headcount needed</v>
+        <v>Percentage of revenue</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Staff Hired</v>
+        <v>B2C Split</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="C10" t="str">
-        <v>Current headcount</v>
+        <v>Percentage of revenue</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Website Status</v>
-      </c>
-      <c r="B11" t="str">
-        <v>In Development</v>
+        <v>Staff Required</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
       </c>
       <c r="C11" t="str">
-        <v>Options: Not Started, In Development, Live, Planned</v>
+        <v>Total headcount needed</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
+        <v>Staff Hired</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Current headcount</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Website Status</v>
+      </c>
+      <c r="B13" t="str">
+        <v>In Development</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Options: Not Started, In Development, Live, Planned</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
         <v>Inventory System Status</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B14" t="str">
         <v>Planned</v>
       </c>
-      <c r="C12" t="str">
+      <c r="C14" t="str">
         <v>Options: Not Started, In Development, Live, Planned</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: Timeline cards collapsed by default, update warehouse refurb progress
- Timeline cards now collapsed on page load
- Warehouse 'Landlord Refurb In Progress' updated to 25% (3 weeks in)
- Updated notes to reflect refurb has started
</commit_message>
<xml_diff>
--- a/public/data/HOC_Investor_Dashboard_Template.xlsx
+++ b/public/data/HOC_Investor_Dashboard_Template.xlsx
@@ -900,7 +900,7 @@
         <v>2025-09-01</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D4" t="str">
         <v>No</v>
@@ -909,7 +909,7 @@
         <v/>
       </c>
       <c r="F4" t="str">
-        <v>Landlord managing refurbishment</v>
+        <v>Started 3 weeks ago - landlord managing refurbishment</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
fix: Warehouse Refurb milestone with proper in-progress state
- Renamed 'Landlord Refurb In Progress' to 'Warehouse Refurb'
- Fixed milestone icon logic: in-progress shows amber clock, not red warning
- Added 'In Progress' badge to active milestones
- Warehouse Refurb at 15% (started 4 Nov 2024, 4 weeks in)
- Fixed milestone date ordering (Aug → Sept → Nov → Jan)
- Amber highlighting for in-progress items in both timeline and list views
</commit_message>
<xml_diff>
--- a/public/data/HOC_Investor_Dashboard_Template.xlsx
+++ b/public/data/HOC_Investor_Dashboard_Template.xlsx
@@ -877,7 +877,7 @@
         <v>Landlord Refurb Design Approved</v>
       </c>
       <c r="B3" t="str">
-        <v>2024-12-01</v>
+        <v>2024-11-01</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -886,7 +886,7 @@
         <v>Yes</v>
       </c>
       <c r="E3" t="str">
-        <v>2024-11-28</v>
+        <v>2024-10-28</v>
       </c>
       <c r="F3" t="str">
         <v>Specifications agreed</v>
@@ -894,13 +894,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Landlord Refurb In Progress</v>
+        <v>Warehouse Refurb</v>
       </c>
       <c r="B4" t="str">
-        <v>2025-09-01</v>
+        <v>2025-08-01</v>
       </c>
       <c r="C4">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D4" t="str">
         <v>No</v>
@@ -909,7 +909,7 @@
         <v/>
       </c>
       <c r="F4" t="str">
-        <v>Started 3 weeks ago - landlord managing refurbishment</v>
+        <v>Started 4 Nov 2024 - landlord managing refurbishment (4 weeks in)</v>
       </c>
     </row>
     <row r="5">
@@ -917,7 +917,7 @@
         <v>Internal Fit-out Planning</v>
       </c>
       <c r="B5" t="str">
-        <v>2025-08-01</v>
+        <v>2025-09-01</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -929,7 +929,7 @@
         <v/>
       </c>
       <c r="F5" t="str">
-        <v>Racking layout design</v>
+        <v>Racking layout design - begins as refurb nears completion</v>
       </c>
     </row>
     <row r="6">
@@ -937,7 +937,7 @@
         <v>Racking &amp; Storage Installed</v>
       </c>
       <c r="B6" t="str">
-        <v>2025-12-01</v>
+        <v>2025-11-15</v>
       </c>
       <c r="C6">
         <v>0</v>

</xml_diff>

<commit_message>
fix: Update all dates for Dec 2025 timeline
- Current date: 2nd December 2025
- Warehouse Refurb started 4 Nov 2025 (4 weeks ago)
- Warehouse target: July 2026
- Showroom target: July 2026 (paused)
- All milestone dates updated to realistic 2025-2026 timeline
</commit_message>
<xml_diff>
--- a/public/data/HOC_Investor_Dashboard_Template.xlsx
+++ b/public/data/HOC_Investor_Dashboard_Template.xlsx
@@ -695,7 +695,7 @@
         <v>Lease Agreement Signed</v>
       </c>
       <c r="B2" t="str">
-        <v>2024-11-01</v>
+        <v>2025-03-01</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -704,7 +704,7 @@
         <v>Yes</v>
       </c>
       <c r="E2" t="str">
-        <v>2024-10-28</v>
+        <v>2025-02-25</v>
       </c>
       <c r="F2" t="str">
         <v>Completed ahead of schedule</v>
@@ -715,7 +715,7 @@
         <v>Design Plans Approved</v>
       </c>
       <c r="B3" t="str">
-        <v>2024-12-15</v>
+        <v>2025-05-15</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -724,7 +724,7 @@
         <v>Yes</v>
       </c>
       <c r="E3" t="str">
-        <v>2024-12-10</v>
+        <v>2025-05-10</v>
       </c>
       <c r="F3" t="str">
         <v>Final designs signed off</v>
@@ -735,10 +735,10 @@
         <v>Contractor Appointed</v>
       </c>
       <c r="B4" t="str">
-        <v>2025-01-15</v>
+        <v>2025-07-15</v>
       </c>
       <c r="C4">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D4" t="str">
         <v>No</v>
@@ -747,7 +747,7 @@
         <v/>
       </c>
       <c r="F4" t="str">
-        <v>Final quotes being reviewed</v>
+        <v>Paused - reviewing options</v>
       </c>
     </row>
     <row r="5">
@@ -755,7 +755,7 @@
         <v>Fit-out Commences</v>
       </c>
       <c r="B5" t="str">
-        <v>2025-02-01</v>
+        <v>2026-03-01</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -767,7 +767,7 @@
         <v/>
       </c>
       <c r="F5" t="str">
-        <v>Awaiting contractor selection</v>
+        <v>On hold pending strategic review</v>
       </c>
     </row>
     <row r="6">
@@ -775,7 +775,7 @@
         <v>Fixtures &amp; Displays Installed</v>
       </c>
       <c r="B6" t="str">
-        <v>2025-04-15</v>
+        <v>2026-05-15</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -787,7 +787,7 @@
         <v/>
       </c>
       <c r="F6" t="str">
-        <v>Custom displays ordered</v>
+        <v>Custom displays to be ordered</v>
       </c>
     </row>
     <row r="7">
@@ -795,7 +795,7 @@
         <v>Showroom Launch</v>
       </c>
       <c r="B7" t="str">
-        <v>2025-06-01</v>
+        <v>2026-07-01</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -807,7 +807,7 @@
         <v/>
       </c>
       <c r="F7" t="str">
-        <v>Target opening date</v>
+        <v>Revised target date</v>
       </c>
     </row>
   </sheetData>
@@ -857,7 +857,7 @@
         <v>Lease Agreement Signed</v>
       </c>
       <c r="B2" t="str">
-        <v>2024-10-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -866,7 +866,7 @@
         <v>Yes</v>
       </c>
       <c r="E2" t="str">
-        <v>2024-09-25</v>
+        <v>2025-05-28</v>
       </c>
       <c r="F2" t="str">
         <v>Long-term lease secured</v>
@@ -877,7 +877,7 @@
         <v>Landlord Refurb Design Approved</v>
       </c>
       <c r="B3" t="str">
-        <v>2024-11-01</v>
+        <v>2025-09-01</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -886,7 +886,7 @@
         <v>Yes</v>
       </c>
       <c r="E3" t="str">
-        <v>2024-10-28</v>
+        <v>2025-08-25</v>
       </c>
       <c r="F3" t="str">
         <v>Specifications agreed</v>
@@ -897,7 +897,7 @@
         <v>Warehouse Refurb</v>
       </c>
       <c r="B4" t="str">
-        <v>2025-08-01</v>
+        <v>2026-04-01</v>
       </c>
       <c r="C4">
         <v>15</v>
@@ -909,7 +909,7 @@
         <v/>
       </c>
       <c r="F4" t="str">
-        <v>Started 4 Nov 2024 - landlord managing refurbishment (4 weeks in)</v>
+        <v>Started 4 Nov 2025 - landlord managing refurbishment (4 weeks in)</v>
       </c>
     </row>
     <row r="5">
@@ -917,7 +917,7 @@
         <v>Internal Fit-out Planning</v>
       </c>
       <c r="B5" t="str">
-        <v>2025-09-01</v>
+        <v>2026-05-01</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -937,7 +937,7 @@
         <v>Racking &amp; Storage Installed</v>
       </c>
       <c r="B6" t="str">
-        <v>2025-11-15</v>
+        <v>2026-06-15</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -957,7 +957,7 @@
         <v>Warehouse Operational</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-15</v>
+        <v>2026-07-15</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1588,7 +1588,7 @@
         <v>Showroom Target Date</v>
       </c>
       <c r="B3" t="str">
-        <v>2025-06-01</v>
+        <v>2026-07-01</v>
       </c>
       <c r="C3" t="str">
         <v>Target completion</v>
@@ -1621,7 +1621,7 @@
         <v>Warehouse Target Date</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-15</v>
+        <v>2026-07-15</v>
       </c>
       <c r="C6" t="str">
         <v>Target completion</v>

</xml_diff>

<commit_message>
fix: Warehouse refurb target Jan 2026, operational Apr 2026
</commit_message>
<xml_diff>
--- a/public/data/HOC_Investor_Dashboard_Template.xlsx
+++ b/public/data/HOC_Investor_Dashboard_Template.xlsx
@@ -897,7 +897,7 @@
         <v>Warehouse Refurb</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-04-01</v>
+        <v>2026-01-15</v>
       </c>
       <c r="C4">
         <v>15</v>
@@ -917,7 +917,7 @@
         <v>Internal Fit-out Planning</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-05-01</v>
+        <v>2026-02-15</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -937,7 +937,7 @@
         <v>Racking &amp; Storage Installed</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-06-15</v>
+        <v>2026-03-15</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -957,7 +957,7 @@
         <v>Warehouse Operational</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-07-15</v>
+        <v>2026-04-15</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1621,7 +1621,7 @@
         <v>Warehouse Target Date</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-07-15</v>
+        <v>2026-04-15</v>
       </c>
       <c r="C6" t="str">
         <v>Target completion</v>

</xml_diff>

<commit_message>
fix: Simplify pause message to 'Project currently on hold'
</commit_message>
<xml_diff>
--- a/public/data/HOC_Investor_Dashboard_Template.xlsx
+++ b/public/data/HOC_Investor_Dashboard_Template.xlsx
@@ -767,7 +767,7 @@
         <v/>
       </c>
       <c r="F5" t="str">
-        <v>On hold pending strategic review</v>
+        <v>On hold</v>
       </c>
     </row>
     <row r="6">
@@ -1602,7 +1602,7 @@
         <v>Yes</v>
       </c>
       <c r="C4" t="str">
-        <v>Project currently on hold pending strategic review</v>
+        <v>Project currently on hold</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
feat: Major financial update with real HOC data
CAPITAL:
- Total raised: £625,000
- Currently deployed: £0 (awaiting landlord handover)
- Next major payment: £245,176 on Dec 19th

WAREHOUSE:
- Landlord handover: Dec 19th, 2025
- Operational from handover date
- First payment breakdown: rent deposit, Q1 rent, service charge, insurance, business rates, legal

SHOWROOM:
- Target: June 2026
- Contractor appointed ✓
- 1st fix in progress (current standstill)
- 1st fix completion: ~1.5 months
- 2nd fix: TBC

NEW CASH FLOW PANEL:
- Monthly outgoings projection
- Closing balance each month
- Expandable payment details
- Burn rate tracking
- Runway calculation

Updated all milestones, costs, and projections to reflect actual HOC data
</commit_message>
<xml_diff>
--- a/public/data/HOC_Investor_Dashboard_Template.xlsx
+++ b/public/data/HOC_Investor_Dashboard_Template.xlsx
@@ -10,7 +10,8 @@
     <sheet name="Suppliers" sheetId="5" r:id="rId5"/>
     <sheet name="Financial_Projections" sheetId="6" r:id="rId6"/>
     <sheet name="Risks_Issues" sheetId="7" r:id="rId7"/>
-    <sheet name="Settings" sheetId="8" r:id="rId8"/>
+    <sheet name="Monthly_Cashflow" sheetId="8" r:id="rId8"/>
+    <sheet name="Settings" sheetId="9" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
@@ -404,14 +405,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="40.83203125" customWidth="1"/>
+    <col min="3" max="3" width="55.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -430,10 +431,10 @@
         <v>Total Capital Raised</v>
       </c>
       <c r="B2">
-        <v>250000</v>
+        <v>625000</v>
       </c>
       <c r="C2" t="str">
-        <v>Seed round from angel investors</v>
+        <v>Total investment secured</v>
       </c>
     </row>
     <row r="3">
@@ -441,10 +442,10 @@
         <v>Capital Deployed</v>
       </c>
       <c r="B3">
-        <v>87500</v>
+        <v>0</v>
       </c>
       <c r="C3" t="str">
-        <v>As of current date</v>
+        <v>No payments made yet - awaiting landlord handover</v>
       </c>
     </row>
     <row r="4">
@@ -452,10 +453,10 @@
         <v>Capital Remaining</v>
       </c>
       <c r="B4">
-        <v>162500</v>
+        <v>625000</v>
       </c>
       <c r="C4" t="str">
-        <v>Available for deployment</v>
+        <v>Full amount available</v>
       </c>
     </row>
     <row r="5">
@@ -463,10 +464,10 @@
         <v>Monthly Burn Rate</v>
       </c>
       <c r="B5">
-        <v>12500</v>
+        <v>17000</v>
       </c>
       <c r="C5" t="str">
-        <v>Average monthly expenditure</v>
+        <v>Estimated ongoing monthly costs after initial setup</v>
       </c>
     </row>
     <row r="6">
@@ -474,7 +475,7 @@
         <v>Runway (Months)</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C6" t="str">
         <v>Calculated from remaining/burn rate</v>
@@ -485,31 +486,42 @@
         <v>Next Major Expense</v>
       </c>
       <c r="B7">
-        <v>75000</v>
+        <v>245176</v>
       </c>
       <c r="C7" t="str">
-        <v>First Stock Order - China Suppliers</v>
+        <v>Due on landlord handover (Dec 19th)</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Next Expense Description</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Warehouse Initial Payment</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Rent deposit, Q1 rent, service charge, insurance, business rates, legal</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
-    <col min="5" max="5" width="40.83203125" customWidth="1"/>
+    <col min="5" max="5" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -531,131 +543,347 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Showroom Fit-out</v>
+        <v>Warehouse - Rent Deposit (7 months)</v>
       </c>
       <c r="B2">
-        <v>65000</v>
+        <v>179743</v>
       </c>
       <c r="C2">
-        <v>22000</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>62000</v>
+        <v>179743</v>
       </c>
       <c r="E2" t="str">
-        <v>Design and construction</v>
+        <v>£128,388 + VAT - Due Dec 19th</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Warehouse Setup</v>
+        <v>Warehouse - Q1 Rent</v>
       </c>
       <c r="B3">
-        <v>40000</v>
+        <v>38516</v>
       </c>
       <c r="C3">
-        <v>8000</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>38000</v>
+        <v>38516</v>
       </c>
       <c r="E3" t="str">
-        <v>Racking, systems, initial setup</v>
+        <v>£32,097 + VAT - Due Dec 19th</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Initial Stock</v>
+        <v>Warehouse - Service Charge (Quarterly)</v>
       </c>
       <c r="B4">
-        <v>75000</v>
+        <v>12000</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>75000</v>
+        <v>48000</v>
       </c>
       <c r="E4" t="str">
-        <v>First order from China suppliers</v>
+        <v>£12,000 per quarter</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Legal &amp; Professional</v>
+        <v>Warehouse - Insurance (Annual)</v>
       </c>
       <c r="B5">
-        <v>15000</v>
+        <v>4800</v>
       </c>
       <c r="C5">
-        <v>12500</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>14000</v>
+        <v>4800</v>
       </c>
       <c r="E5" t="str">
-        <v>Company formation, contracts, accounting</v>
+        <v>Yearly upfront - Due Dec 19th</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Marketing &amp; Launch</v>
+        <v>Warehouse - Business Rates (Monthly)</v>
       </c>
       <c r="B6">
-        <v>25000</v>
+        <v>5000</v>
       </c>
       <c r="C6">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>25000</v>
+        <v>60000</v>
       </c>
       <c r="E6" t="str">
-        <v>Brand, website, launch campaign</v>
+        <v>£5,000 per month</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Technology &amp; Systems</v>
+        <v>Warehouse - Legal/Professional</v>
       </c>
       <c r="B7">
-        <v>12000</v>
+        <v>13117</v>
       </c>
       <c r="C7">
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>11000</v>
+        <v>13117</v>
       </c>
       <c r="E7" t="str">
-        <v>POS, inventory, website</v>
+        <v>£10,930.5 + VAT - Due Dec 19th</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
+        <v>Warehouse - Racking &amp; Setup</v>
+      </c>
+      <c r="B8">
+        <v>25000</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>25000</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Post-handover setup</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Showroom - Total Completion</v>
+      </c>
+      <c r="B9">
+        <v>255000</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>255000</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Estimate to complete showroom</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
         <v>Working Capital</v>
       </c>
-      <c r="B8">
-        <v>18000</v>
-      </c>
-      <c r="C8">
-        <v>34000</v>
-      </c>
-      <c r="D8">
-        <v>40000</v>
-      </c>
-      <c r="E8" t="str">
-        <v>Operating expenses, contingency</v>
+      <c r="B10">
+        <v>50000</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>50000</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Operating expenses reserve</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E10"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="50.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Milestone</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Target Date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Status %</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Complete</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Actual Date</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Lease Agreement Signed</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2025-03-01</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2025-02-25</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Completed</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Landlord Scope Complete</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2025-04-30</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2025-04-15</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Landlord finished his works</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Contractor Appointed</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2025-06-01</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2025-05-20</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Contractor selected and appointed</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>1st Fix In Progress</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2026-01-15</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5" t="str">
+        <v>No</v>
+      </c>
+      <c r="E5" t="str">
+        <v/>
+      </c>
+      <c r="F5" t="str">
+        <v>Currently on standstill - expected complete in 1.5 months</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>2nd Fix</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2026-03-01</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="str">
+        <v>No</v>
+      </c>
+      <c r="E6" t="str">
+        <v/>
+      </c>
+      <c r="F6" t="str">
+        <v>TBC - follows 1st fix completion</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Fixtures &amp; Displays</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2026-05-01</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="str">
+        <v>No</v>
+      </c>
+      <c r="E7" t="str">
+        <v/>
+      </c>
+      <c r="F7" t="str">
+        <v>Final installations</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Showroom Launch</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2026-06-01</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="str">
+        <v>No</v>
+      </c>
+      <c r="E8" t="str">
+        <v/>
+      </c>
+      <c r="F8" t="str">
+        <v>Target opening date</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:F8"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -667,7 +895,7 @@
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="30.83203125" customWidth="1"/>
+    <col min="6" max="6" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -695,168 +923,6 @@
         <v>Lease Agreement Signed</v>
       </c>
       <c r="B2" t="str">
-        <v>2025-03-01</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="E2" t="str">
-        <v>2025-02-25</v>
-      </c>
-      <c r="F2" t="str">
-        <v>Completed ahead of schedule</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Design Plans Approved</v>
-      </c>
-      <c r="B3" t="str">
-        <v>2025-05-15</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="E3" t="str">
-        <v>2025-05-10</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Final designs signed off</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Contractor Appointed</v>
-      </c>
-      <c r="B4" t="str">
-        <v>2025-07-15</v>
-      </c>
-      <c r="C4">
-        <v>50</v>
-      </c>
-      <c r="D4" t="str">
-        <v>No</v>
-      </c>
-      <c r="E4" t="str">
-        <v/>
-      </c>
-      <c r="F4" t="str">
-        <v>Paused - reviewing options</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Fit-out Commences</v>
-      </c>
-      <c r="B5" t="str">
-        <v>2026-03-01</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" t="str">
-        <v>No</v>
-      </c>
-      <c r="E5" t="str">
-        <v/>
-      </c>
-      <c r="F5" t="str">
-        <v>On hold</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Fixtures &amp; Displays Installed</v>
-      </c>
-      <c r="B6" t="str">
-        <v>2026-05-15</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6" t="str">
-        <v>No</v>
-      </c>
-      <c r="E6" t="str">
-        <v/>
-      </c>
-      <c r="F6" t="str">
-        <v>Custom displays to be ordered</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Showroom Launch</v>
-      </c>
-      <c r="B7" t="str">
-        <v>2026-07-01</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" t="str">
-        <v>No</v>
-      </c>
-      <c r="E7" t="str">
-        <v/>
-      </c>
-      <c r="F7" t="str">
-        <v>Revised target date</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <cols>
-    <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="30.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Milestone</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Target Date</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Status %</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Complete</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Actual Date</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Notes</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Lease Agreement Signed</v>
-      </c>
-      <c r="B2" t="str">
         <v>2025-06-01</v>
       </c>
       <c r="C2">
@@ -897,10 +963,10 @@
         <v>Warehouse Refurb</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-15</v>
+        <v>2025-12-19</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="D4" t="str">
         <v>No</v>
@@ -909,15 +975,15 @@
         <v/>
       </c>
       <c r="F4" t="str">
-        <v>Started 4 Nov 2025 - landlord managing refurbishment (4 weeks in)</v>
+        <v>Landlord refurb in progress - handover Dec 19th</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Internal Fit-out Planning</v>
+        <v>Landlord Handover</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-02-15</v>
+        <v>2025-12-19</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -929,15 +995,15 @@
         <v/>
       </c>
       <c r="F5" t="str">
-        <v>Racking layout design - begins as refurb nears completion</v>
+        <v>Warehouse becomes operational</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Racking &amp; Storage Installed</v>
+        <v>Racking &amp; Setup</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-03-15</v>
+        <v>2026-01-15</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -949,15 +1015,15 @@
         <v/>
       </c>
       <c r="F6" t="str">
-        <v>Industrial racking system</v>
+        <v>Internal setup after handover</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Warehouse Operational</v>
+        <v>Warehouse Fully Operational</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-04-15</v>
+        <v>2026-01-31</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -969,7 +1035,7 @@
         <v/>
       </c>
       <c r="F7" t="str">
-        <v>Target go-live date</v>
+        <v>All systems ready</v>
       </c>
     </row>
   </sheetData>
@@ -1332,7 +1398,7 @@
     <col min="2" max="2" width="25.83203125" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" customWidth="1"/>
     <col min="4" max="4" width="45.83203125" customWidth="1"/>
-    <col min="5" max="5" width="50.83203125" customWidth="1"/>
+    <col min="5" max="5" width="45.83203125" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" customWidth="1"/>
@@ -1373,22 +1439,22 @@
         <v>R001</v>
       </c>
       <c r="B2" t="str">
-        <v>Supplier Lead Times</v>
+        <v>Showroom 1st Fix Delay</v>
       </c>
       <c r="C2" t="str">
         <v>Amber</v>
       </c>
       <c r="D2" t="str">
-        <v>Chinese New Year may impact initial stock delivery timeline</v>
+        <v>Current standstill on 1st fix works</v>
       </c>
       <c r="E2" t="str">
-        <v>Planning stock order 6 weeks before CNY. Multiple supplier relationships.</v>
+        <v>Monitoring closely - expected to resume shortly</v>
       </c>
       <c r="F2" t="str">
         <v>Open</v>
       </c>
       <c r="G2" t="str">
-        <v>Operations</v>
+        <v>Project Lead</v>
       </c>
       <c r="H2" t="str">
         <v>No</v>
@@ -1402,16 +1468,16 @@
         <v>R002</v>
       </c>
       <c r="B3" t="str">
-        <v>Warehouse Refurb Delay</v>
+        <v>Warehouse Handover Timing</v>
       </c>
       <c r="C3" t="str">
-        <v>Amber</v>
+        <v>Green</v>
       </c>
       <c r="D3" t="str">
-        <v>Landlord refurbishment timeline dependent on contractor availability</v>
+        <v>Landlord confirmed Dec 19th handover</v>
       </c>
       <c r="E3" t="str">
-        <v>Weekly progress calls with landlord. Contingency storage identified.</v>
+        <v>Date confirmed - preparing for handover</v>
       </c>
       <c r="F3" t="str">
         <v>Open</v>
@@ -1431,22 +1497,22 @@
         <v>R003</v>
       </c>
       <c r="B4" t="str">
-        <v>Import Duties Post-Brexit</v>
+        <v>Supplier Lead Times</v>
       </c>
       <c r="C4" t="str">
-        <v>Green</v>
+        <v>Amber</v>
       </c>
       <c r="D4" t="str">
-        <v>Potential changes to UK import regulations</v>
+        <v>Chinese New Year may impact initial stock delivery</v>
       </c>
       <c r="E4" t="str">
-        <v>Working with customs broker. Duty calculations built into pricing model.</v>
+        <v>Planning stock order ahead of CNY</v>
       </c>
       <c r="F4" t="str">
         <v>Open</v>
       </c>
       <c r="G4" t="str">
-        <v>Finance</v>
+        <v>Operations</v>
       </c>
       <c r="H4" t="str">
         <v>No</v>
@@ -1460,28 +1526,28 @@
         <v>R004</v>
       </c>
       <c r="B5" t="str">
-        <v>Showroom Contractor Selection</v>
+        <v>Currency Fluctuation</v>
       </c>
       <c r="C5" t="str">
         <v>Amber</v>
       </c>
       <c r="D5" t="str">
-        <v>Final contractor decision pending - 3 quotes received</v>
+        <v>GBP/CNY exchange rate volatility</v>
       </c>
       <c r="E5" t="str">
-        <v>Expediting final meetings. Budget allows for preferred contractor.</v>
+        <v>Building 5% currency buffer into pricing</v>
       </c>
       <c r="F5" t="str">
         <v>Open</v>
       </c>
       <c r="G5" t="str">
-        <v>Project Lead</v>
+        <v>Finance</v>
       </c>
       <c r="H5" t="str">
         <v>No</v>
       </c>
       <c r="I5" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
     </row>
     <row r="6">
@@ -1489,16 +1555,16 @@
         <v>R005</v>
       </c>
       <c r="B6" t="str">
-        <v>Currency Fluctuation</v>
+        <v>Cash Flow Management</v>
       </c>
       <c r="C6" t="str">
-        <v>Amber</v>
+        <v>Green</v>
       </c>
       <c r="D6" t="str">
-        <v>GBP/CNY exchange rate volatility affects stock costs</v>
+        <v>Large initial payment due Dec 19th</v>
       </c>
       <c r="E6" t="str">
-        <v>Building 5% currency buffer into pricing. Considering forward contracts.</v>
+        <v>Capital secured and available</v>
       </c>
       <c r="F6" t="str">
         <v>Open</v>
@@ -1524,10 +1590,10 @@
         <v>Green</v>
       </c>
       <c r="D7" t="str">
-        <v>Need to hire showroom manager and warehouse staff</v>
+        <v>Need to hire warehouse and showroom staff</v>
       </c>
       <c r="E7" t="str">
-        <v>Recruitment to begin Q1 2025. Job specs prepared.</v>
+        <v>Recruitment to begin Q1 2026</v>
       </c>
       <c r="F7" t="str">
         <v>Open</v>
@@ -1551,14 +1617,273 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Month</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Item</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Amount</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Running Balance</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Opening</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Capital Raised</v>
+      </c>
+      <c r="C2">
+        <v>625000</v>
+      </c>
+      <c r="D2">
+        <v>625000</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Starting balance</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Dec 2025</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Legal/Professional Fees</v>
+      </c>
+      <c r="C3">
+        <v>-13117</v>
+      </c>
+      <c r="D3">
+        <v>611883</v>
+      </c>
+      <c r="E3" t="str">
+        <v>£10,930.5 + VAT</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Dec 2025</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Rent Deposit (7 months)</v>
+      </c>
+      <c r="C4">
+        <v>-179743</v>
+      </c>
+      <c r="D4">
+        <v>432140</v>
+      </c>
+      <c r="E4" t="str">
+        <v>£128,388 + VAT</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Dec 2025</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Q1 Rent</v>
+      </c>
+      <c r="C5">
+        <v>-38516</v>
+      </c>
+      <c r="D5">
+        <v>393624</v>
+      </c>
+      <c r="E5" t="str">
+        <v>£32,097 + VAT</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Dec 2025</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Service Charge (Q1)</v>
+      </c>
+      <c r="C6">
+        <v>-12000</v>
+      </c>
+      <c r="D6">
+        <v>381624</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Quarterly payment</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Dec 2025</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Insurance (Annual)</v>
+      </c>
+      <c r="C7">
+        <v>-4800</v>
+      </c>
+      <c r="D7">
+        <v>376824</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Yearly upfront</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Dec 2025</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Business Rates</v>
+      </c>
+      <c r="C8">
+        <v>-5000</v>
+      </c>
+      <c r="D8">
+        <v>371824</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Monthly payment</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Jan 2026</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Business Rates</v>
+      </c>
+      <c r="C9">
+        <v>-5000</v>
+      </c>
+      <c r="D9">
+        <v>366824</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Monthly payment</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Jan 2026</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Racking &amp; Setup</v>
+      </c>
+      <c r="C10">
+        <v>-25000</v>
+      </c>
+      <c r="D10">
+        <v>341824</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Warehouse internal setup</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Feb 2026</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Business Rates</v>
+      </c>
+      <c r="C11">
+        <v>-5000</v>
+      </c>
+      <c r="D11">
+        <v>336824</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Monthly payment</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Mar 2026</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Business Rates</v>
+      </c>
+      <c r="C12">
+        <v>-5000</v>
+      </c>
+      <c r="D12">
+        <v>331824</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Monthly payment</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Mar 2026</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Q2 Rent</v>
+      </c>
+      <c r="C13">
+        <v>-38516</v>
+      </c>
+      <c r="D13">
+        <v>293308</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Quarterly rent</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Mar 2026</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Service Charge (Q2)</v>
+      </c>
+      <c r="C14">
+        <v>-12000</v>
+      </c>
+      <c r="D14">
+        <v>281308</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Quarterly payment</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E14"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="40.83203125" customWidth="1"/>
+    <col min="3" max="3" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1588,7 +1913,7 @@
         <v>Showroom Target Date</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-07-01</v>
+        <v>2026-06-01</v>
       </c>
       <c r="C3" t="str">
         <v>Target completion</v>
@@ -1599,10 +1924,10 @@
         <v>Showroom Paused</v>
       </c>
       <c r="B4" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="C4" t="str">
-        <v>Project currently on hold</v>
+        <v>Active - 1st fix in progress</v>
       </c>
     </row>
     <row r="5">
@@ -1621,10 +1946,10 @@
         <v>Warehouse Target Date</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-04-15</v>
+        <v>2026-01-31</v>
       </c>
       <c r="C6" t="str">
-        <v>Target completion</v>
+        <v>Target fully operational</v>
       </c>
     </row>
     <row r="7">
@@ -1640,32 +1965,32 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Gross Margin Target</v>
-      </c>
-      <c r="B8">
-        <v>45</v>
+        <v>Warehouse Handover Date</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2025-12-19</v>
       </c>
       <c r="C8" t="str">
-        <v>Percentage</v>
+        <v>Landlord handover date</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>B2B Split</v>
+        <v>Gross Margin Target</v>
       </c>
       <c r="B9">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C9" t="str">
-        <v>Percentage of revenue</v>
+        <v>Percentage</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>B2C Split</v>
+        <v>B2B Split</v>
       </c>
       <c r="B10">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C10" t="str">
         <v>Percentage of revenue</v>
@@ -1673,51 +1998,62 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Staff Required</v>
+        <v>B2C Split</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="C11" t="str">
-        <v>Total headcount needed</v>
+        <v>Percentage of revenue</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Staff Hired</v>
+        <v>Staff Required</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" t="str">
-        <v>Current headcount</v>
+        <v>Total headcount needed</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Website Status</v>
-      </c>
-      <c r="B13" t="str">
-        <v>In Development</v>
+        <v>Staff Hired</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
       </c>
       <c r="C13" t="str">
-        <v>Options: Not Started, In Development, Live, Planned</v>
+        <v>Current headcount</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Inventory System Status</v>
+        <v>Website Status</v>
       </c>
       <c r="B14" t="str">
-        <v>Planned</v>
+        <v>In Development</v>
       </c>
       <c r="C14" t="str">
         <v>Options: Not Started, In Development, Live, Planned</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Inventory System Status</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Planned</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Options: Not Started, In Development, Live, Planned</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Add VAT breakdown to cash flow panel
- Shows Net, VAT, and Gross amounts for each payment
- VAT Reclaimable badge on eligible items
- Total VAT reclaimable summary card
- December payment breakdown:
  * Legal: £10,930.50 + VAT = £13,116.60
  * Rent Deposit: £128,388 + VAT = £154,065.60
  * Q1 Rent: £32,097 + VAT = £38,516.40
  * Service Charge: £12,000 (no VAT)
  * Insurance: £4,800 (exempt)
  * Business Rates: £5,000 (no VAT)
- Updated Excel template with VAT columns
</commit_message>
<xml_diff>
--- a/public/data/HOC_Investor_Dashboard_Template.xlsx
+++ b/public/data/HOC_Investor_Dashboard_Template.xlsx
@@ -1617,7 +1617,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1625,8 +1625,11 @@
     <col min="1" max="1" width="12.83203125" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="25.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1637,12 +1640,21 @@
         <v>Item</v>
       </c>
       <c r="C1" t="str">
-        <v>Amount</v>
+        <v>Net Amount</v>
       </c>
       <c r="D1" t="str">
+        <v>VAT (20%)</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Gross Amount</v>
+      </c>
+      <c r="F1" t="str">
+        <v>VAT Reclaimable</v>
+      </c>
+      <c r="G1" t="str">
         <v>Running Balance</v>
       </c>
-      <c r="E1" t="str">
+      <c r="H1" t="str">
         <v>Notes</v>
       </c>
     </row>
@@ -1657,9 +1669,18 @@
         <v>625000</v>
       </c>
       <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>625000</v>
       </c>
-      <c r="E2" t="str">
+      <c r="F2" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G2">
+        <v>625000</v>
+      </c>
+      <c r="H2" t="str">
         <v>Starting balance</v>
       </c>
     </row>
@@ -1671,13 +1692,22 @@
         <v>Legal/Professional Fees</v>
       </c>
       <c r="C3">
-        <v>-13117</v>
+        <v>10930.5</v>
       </c>
       <c r="D3">
-        <v>611883</v>
-      </c>
-      <c r="E3" t="str">
-        <v>£10,930.5 + VAT</v>
+        <v>2186.1</v>
+      </c>
+      <c r="E3">
+        <v>13116.6</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G3">
+        <v>611883.4</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Legal and professional fees</v>
       </c>
     </row>
     <row r="4">
@@ -1688,13 +1718,22 @@
         <v>Rent Deposit (7 months)</v>
       </c>
       <c r="C4">
-        <v>-179743</v>
+        <v>128388</v>
       </c>
       <c r="D4">
-        <v>432140</v>
-      </c>
-      <c r="E4" t="str">
-        <v>£128,388 + VAT</v>
+        <v>25677.6</v>
+      </c>
+      <c r="E4">
+        <v>154065.6</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G4">
+        <v>457817.8</v>
+      </c>
+      <c r="H4" t="str">
+        <v>7 months deposit</v>
       </c>
     </row>
     <row r="5">
@@ -1705,13 +1744,22 @@
         <v>Q1 Rent</v>
       </c>
       <c r="C5">
-        <v>-38516</v>
+        <v>32097</v>
       </c>
       <c r="D5">
-        <v>393624</v>
-      </c>
-      <c r="E5" t="str">
-        <v>£32,097 + VAT</v>
+        <v>6419.4</v>
+      </c>
+      <c r="E5">
+        <v>38516.4</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G5">
+        <v>419301.4</v>
+      </c>
+      <c r="H5" t="str">
+        <v>Quarter 1 rent payment</v>
       </c>
     </row>
     <row r="6">
@@ -1722,13 +1770,22 @@
         <v>Service Charge (Q1)</v>
       </c>
       <c r="C6">
-        <v>-12000</v>
+        <v>12000</v>
       </c>
       <c r="D6">
-        <v>381624</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Quarterly payment</v>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>12000</v>
+      </c>
+      <c r="F6" t="str">
+        <v>No</v>
+      </c>
+      <c r="G6">
+        <v>407301.4</v>
+      </c>
+      <c r="H6" t="str">
+        <v>Quarterly service charge - exempt</v>
       </c>
     </row>
     <row r="7">
@@ -1739,13 +1796,22 @@
         <v>Insurance (Annual)</v>
       </c>
       <c r="C7">
-        <v>-4800</v>
+        <v>4800</v>
       </c>
       <c r="D7">
-        <v>376824</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Yearly upfront</v>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>4800</v>
+      </c>
+      <c r="F7" t="str">
+        <v>No</v>
+      </c>
+      <c r="G7">
+        <v>402501.4</v>
+      </c>
+      <c r="H7" t="str">
+        <v>Annual insurance - exempt</v>
       </c>
     </row>
     <row r="8">
@@ -1753,16 +1819,25 @@
         <v>Dec 2025</v>
       </c>
       <c r="B8" t="str">
-        <v>Business Rates</v>
+        <v>Business Rates (Dec)</v>
       </c>
       <c r="C8">
-        <v>-5000</v>
+        <v>5000</v>
       </c>
       <c r="D8">
-        <v>371824</v>
-      </c>
-      <c r="E8" t="str">
-        <v>Monthly payment</v>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>5000</v>
+      </c>
+      <c r="F8" t="str">
+        <v>No</v>
+      </c>
+      <c r="G8">
+        <v>397501.4</v>
+      </c>
+      <c r="H8" t="str">
+        <v>Monthly - no VAT on rates</v>
       </c>
     </row>
     <row r="9">
@@ -1773,12 +1848,21 @@
         <v>Business Rates</v>
       </c>
       <c r="C9">
-        <v>-5000</v>
+        <v>5000</v>
       </c>
       <c r="D9">
-        <v>366824</v>
-      </c>
-      <c r="E9" t="str">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>5000</v>
+      </c>
+      <c r="F9" t="str">
+        <v>No</v>
+      </c>
+      <c r="G9">
+        <v>392501.4</v>
+      </c>
+      <c r="H9" t="str">
         <v>Monthly payment</v>
       </c>
     </row>
@@ -1790,46 +1874,73 @@
         <v>Racking &amp; Setup</v>
       </c>
       <c r="C10">
-        <v>-25000</v>
+        <v>20833.33</v>
       </c>
       <c r="D10">
-        <v>341824</v>
-      </c>
-      <c r="E10" t="str">
-        <v>Warehouse internal setup</v>
+        <v>4166.67</v>
+      </c>
+      <c r="E10">
+        <v>25000</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G10">
+        <v>367501.4</v>
+      </c>
+      <c r="H10" t="str">
+        <v>Warehouse racking installation</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Feb 2026</v>
+        <v>Jan 2026</v>
       </c>
       <c r="B11" t="str">
-        <v>Business Rates</v>
+        <v>Warehouse Equipment</v>
       </c>
       <c r="C11">
-        <v>-5000</v>
+        <v>4166.67</v>
       </c>
       <c r="D11">
-        <v>336824</v>
-      </c>
-      <c r="E11" t="str">
-        <v>Monthly payment</v>
+        <v>833.33</v>
+      </c>
+      <c r="E11">
+        <v>5000</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G11">
+        <v>362501.4</v>
+      </c>
+      <c r="H11" t="str">
+        <v>Initial equipment</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Mar 2026</v>
+        <v>Feb 2026</v>
       </c>
       <c r="B12" t="str">
         <v>Business Rates</v>
       </c>
       <c r="C12">
-        <v>-5000</v>
+        <v>5000</v>
       </c>
       <c r="D12">
-        <v>331824</v>
-      </c>
-      <c r="E12" t="str">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>5000</v>
+      </c>
+      <c r="F12" t="str">
+        <v>No</v>
+      </c>
+      <c r="G12">
+        <v>357501.4</v>
+      </c>
+      <c r="H12" t="str">
         <v>Monthly payment</v>
       </c>
     </row>
@@ -1838,16 +1949,25 @@
         <v>Mar 2026</v>
       </c>
       <c r="B13" t="str">
-        <v>Q2 Rent</v>
+        <v>Business Rates</v>
       </c>
       <c r="C13">
-        <v>-38516</v>
+        <v>5000</v>
       </c>
       <c r="D13">
-        <v>293308</v>
-      </c>
-      <c r="E13" t="str">
-        <v>Quarterly rent</v>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>5000</v>
+      </c>
+      <c r="F13" t="str">
+        <v>No</v>
+      </c>
+      <c r="G13">
+        <v>352501.4</v>
+      </c>
+      <c r="H13" t="str">
+        <v>Monthly payment</v>
       </c>
     </row>
     <row r="14">
@@ -1855,21 +1975,186 @@
         <v>Mar 2026</v>
       </c>
       <c r="B14" t="str">
+        <v>Q2 Rent</v>
+      </c>
+      <c r="C14">
+        <v>32097</v>
+      </c>
+      <c r="D14">
+        <v>6419.4</v>
+      </c>
+      <c r="E14">
+        <v>38516.4</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G14">
+        <v>313985</v>
+      </c>
+      <c r="H14" t="str">
+        <v>Quarter 2 rent payment</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Mar 2026</v>
+      </c>
+      <c r="B15" t="str">
         <v>Service Charge (Q2)</v>
       </c>
-      <c r="C14">
-        <v>-12000</v>
-      </c>
-      <c r="D14">
-        <v>281308</v>
-      </c>
-      <c r="E14" t="str">
-        <v>Quarterly payment</v>
+      <c r="C15">
+        <v>12000</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>12000</v>
+      </c>
+      <c r="F15" t="str">
+        <v>No</v>
+      </c>
+      <c r="G15">
+        <v>301985</v>
+      </c>
+      <c r="H15" t="str">
+        <v>Quarterly service charge</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Apr 2026</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Business Rates</v>
+      </c>
+      <c r="C16">
+        <v>5000</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>5000</v>
+      </c>
+      <c r="F16" t="str">
+        <v>No</v>
+      </c>
+      <c r="G16">
+        <v>296985</v>
+      </c>
+      <c r="H16" t="str">
+        <v>Monthly payment</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>May 2026</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Business Rates</v>
+      </c>
+      <c r="C17">
+        <v>5000</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>5000</v>
+      </c>
+      <c r="F17" t="str">
+        <v>No</v>
+      </c>
+      <c r="G17">
+        <v>291985</v>
+      </c>
+      <c r="H17" t="str">
+        <v>Monthly payment</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Jun 2026</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Business Rates</v>
+      </c>
+      <c r="C18">
+        <v>5000</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>5000</v>
+      </c>
+      <c r="F18" t="str">
+        <v>No</v>
+      </c>
+      <c r="G18">
+        <v>286985</v>
+      </c>
+      <c r="H18" t="str">
+        <v>Monthly payment</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Jun 2026</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Q3 Rent</v>
+      </c>
+      <c r="C19">
+        <v>32097</v>
+      </c>
+      <c r="D19">
+        <v>6419.4</v>
+      </c>
+      <c r="E19">
+        <v>38516.4</v>
+      </c>
+      <c r="F19" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G19">
+        <v>248468.6</v>
+      </c>
+      <c r="H19" t="str">
+        <v>Quarter 3 rent payment</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Jun 2026</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Service Charge (Q3)</v>
+      </c>
+      <c r="C20">
+        <v>12000</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>12000</v>
+      </c>
+      <c r="F20" t="str">
+        <v>No</v>
+      </c>
+      <c r="G20">
+        <v>236468.6</v>
+      </c>
+      <c r="H20" t="str">
+        <v>Quarterly service charge</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H20"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fix: Remove unconfirmed expenses, keep only guaranteed figures
Removed:
- Racking & Setup (£25,000) from January
- Warehouse Equipment from January
- Working Capital placeholder

Kept only confirmed outgoings:
- Dec 2025: Legal, Rent Deposit, Q1 Rent, Service Charge, Insurance, Business Rates
- Ongoing: Business Rates (monthly), Rent (quarterly), Service Charge (quarterly)
</commit_message>
<xml_diff>
--- a/public/data/HOC_Investor_Dashboard_Template.xlsx
+++ b/public/data/HOC_Investor_Dashboard_Template.xlsx
@@ -512,7 +512,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -546,16 +546,16 @@
         <v>Warehouse - Rent Deposit (7 months)</v>
       </c>
       <c r="B2">
-        <v>179743</v>
+        <v>154065.6</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>179743</v>
+        <v>154065.6</v>
       </c>
       <c r="E2" t="str">
-        <v>£128,388 + VAT - Due Dec 19th</v>
+        <v>£128,388 + VAT (£25,677.60) - Due Dec 19th</v>
       </c>
     </row>
     <row r="3">
@@ -563,16 +563,16 @@
         <v>Warehouse - Q1 Rent</v>
       </c>
       <c r="B3">
-        <v>38516</v>
+        <v>38516.4</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>38516</v>
+        <v>38516.4</v>
       </c>
       <c r="E3" t="str">
-        <v>£32,097 + VAT - Due Dec 19th</v>
+        <v>£32,097 + VAT (£6,419.40) - Due Dec 19th</v>
       </c>
     </row>
     <row r="4">
@@ -589,7 +589,7 @@
         <v>48000</v>
       </c>
       <c r="E4" t="str">
-        <v>£12,000 per quarter</v>
+        <v>£12,000 per quarter - No VAT</v>
       </c>
     </row>
     <row r="5">
@@ -606,7 +606,7 @@
         <v>4800</v>
       </c>
       <c r="E5" t="str">
-        <v>Yearly upfront - Due Dec 19th</v>
+        <v>Yearly upfront - VAT exempt - Due Dec 19th</v>
       </c>
     </row>
     <row r="6">
@@ -623,7 +623,7 @@
         <v>60000</v>
       </c>
       <c r="E6" t="str">
-        <v>£5,000 per month</v>
+        <v>£5,000 per month - No VAT</v>
       </c>
     </row>
     <row r="7">
@@ -631,72 +631,38 @@
         <v>Warehouse - Legal/Professional</v>
       </c>
       <c r="B7">
-        <v>13117</v>
+        <v>13116.6</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>13117</v>
+        <v>13116.6</v>
       </c>
       <c r="E7" t="str">
-        <v>£10,930.5 + VAT - Due Dec 19th</v>
+        <v>£10,930.50 + VAT (£2,186.10) - Due Dec 19th</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Warehouse - Racking &amp; Setup</v>
+        <v>Showroom - Total Completion</v>
       </c>
       <c r="B8">
-        <v>25000</v>
+        <v>255000</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>25000</v>
+        <v>255000</v>
       </c>
       <c r="E8" t="str">
-        <v>Post-handover setup</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Showroom - Total Completion</v>
-      </c>
-      <c r="B9">
-        <v>255000</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>255000</v>
-      </c>
-      <c r="E9" t="str">
         <v>Estimate to complete showroom</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Working Capital</v>
-      </c>
-      <c r="B10">
-        <v>50000</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>50000</v>
-      </c>
-      <c r="E10" t="str">
-        <v>Operating expenses reserve</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1617,7 +1583,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1819,7 +1785,7 @@
         <v>Dec 2025</v>
       </c>
       <c r="B8" t="str">
-        <v>Business Rates (Dec)</v>
+        <v>Business Rates</v>
       </c>
       <c r="C8">
         <v>5000</v>
@@ -1834,7 +1800,7 @@
         <v>No</v>
       </c>
       <c r="G8">
-        <v>397501.4</v>
+        <v>371824</v>
       </c>
       <c r="H8" t="str">
         <v>Monthly - no VAT on rates</v>
@@ -1860,7 +1826,7 @@
         <v>No</v>
       </c>
       <c r="G9">
-        <v>392501.4</v>
+        <v>366824</v>
       </c>
       <c r="H9" t="str">
         <v>Monthly payment</v>
@@ -1868,80 +1834,80 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Jan 2026</v>
+        <v>Feb 2026</v>
       </c>
       <c r="B10" t="str">
-        <v>Racking &amp; Setup</v>
+        <v>Business Rates</v>
       </c>
       <c r="C10">
-        <v>20833.33</v>
+        <v>5000</v>
       </c>
       <c r="D10">
-        <v>4166.67</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>25000</v>
+        <v>5000</v>
       </c>
       <c r="F10" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G10">
-        <v>367501.4</v>
+        <v>361824</v>
       </c>
       <c r="H10" t="str">
-        <v>Warehouse racking installation</v>
+        <v>Monthly payment</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Jan 2026</v>
+        <v>Mar 2026</v>
       </c>
       <c r="B11" t="str">
-        <v>Warehouse Equipment</v>
+        <v>Business Rates</v>
       </c>
       <c r="C11">
-        <v>4166.67</v>
+        <v>5000</v>
       </c>
       <c r="D11">
-        <v>833.33</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>5000</v>
       </c>
       <c r="F11" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G11">
-        <v>362501.4</v>
+        <v>356824</v>
       </c>
       <c r="H11" t="str">
-        <v>Initial equipment</v>
+        <v>Monthly payment</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Feb 2026</v>
+        <v>Mar 2026</v>
       </c>
       <c r="B12" t="str">
-        <v>Business Rates</v>
+        <v>Q2 Rent</v>
       </c>
       <c r="C12">
-        <v>5000</v>
+        <v>32097</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>6419.4</v>
       </c>
       <c r="E12">
-        <v>5000</v>
+        <v>38516.4</v>
       </c>
       <c r="F12" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G12">
-        <v>357501.4</v>
+        <v>318307.6</v>
       </c>
       <c r="H12" t="str">
-        <v>Monthly payment</v>
+        <v>Quarter 2 rent payment</v>
       </c>
     </row>
     <row r="13">
@@ -1949,82 +1915,82 @@
         <v>Mar 2026</v>
       </c>
       <c r="B13" t="str">
-        <v>Business Rates</v>
+        <v>Service Charge (Q2)</v>
       </c>
       <c r="C13">
-        <v>5000</v>
+        <v>12000</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>5000</v>
+        <v>12000</v>
       </c>
       <c r="F13" t="str">
         <v>No</v>
       </c>
       <c r="G13">
-        <v>352501.4</v>
+        <v>306307.6</v>
       </c>
       <c r="H13" t="str">
-        <v>Monthly payment</v>
+        <v>Quarterly service charge</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Mar 2026</v>
+        <v>Apr 2026</v>
       </c>
       <c r="B14" t="str">
-        <v>Q2 Rent</v>
+        <v>Business Rates</v>
       </c>
       <c r="C14">
-        <v>32097</v>
+        <v>5000</v>
       </c>
       <c r="D14">
-        <v>6419.4</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>38516.4</v>
+        <v>5000</v>
       </c>
       <c r="F14" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G14">
-        <v>313985</v>
+        <v>301307.6</v>
       </c>
       <c r="H14" t="str">
-        <v>Quarter 2 rent payment</v>
+        <v>Monthly payment</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Mar 2026</v>
+        <v>May 2026</v>
       </c>
       <c r="B15" t="str">
-        <v>Service Charge (Q2)</v>
+        <v>Business Rates</v>
       </c>
       <c r="C15">
-        <v>12000</v>
+        <v>5000</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>12000</v>
+        <v>5000</v>
       </c>
       <c r="F15" t="str">
         <v>No</v>
       </c>
       <c r="G15">
-        <v>301985</v>
+        <v>296307.6</v>
       </c>
       <c r="H15" t="str">
-        <v>Quarterly service charge</v>
+        <v>Monthly payment</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Apr 2026</v>
+        <v>Jun 2026</v>
       </c>
       <c r="B16" t="str">
         <v>Business Rates</v>
@@ -2042,7 +2008,7 @@
         <v>No</v>
       </c>
       <c r="G16">
-        <v>296985</v>
+        <v>291307.6</v>
       </c>
       <c r="H16" t="str">
         <v>Monthly payment</v>
@@ -2050,28 +2016,28 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>May 2026</v>
+        <v>Jun 2026</v>
       </c>
       <c r="B17" t="str">
-        <v>Business Rates</v>
+        <v>Q3 Rent</v>
       </c>
       <c r="C17">
-        <v>5000</v>
+        <v>32097</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>6419.4</v>
       </c>
       <c r="E17">
-        <v>5000</v>
+        <v>38516.4</v>
       </c>
       <c r="F17" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G17">
-        <v>291985</v>
+        <v>252791.2</v>
       </c>
       <c r="H17" t="str">
-        <v>Monthly payment</v>
+        <v>Quarter 3 rent payment</v>
       </c>
     </row>
     <row r="18">
@@ -2079,82 +2045,30 @@
         <v>Jun 2026</v>
       </c>
       <c r="B18" t="str">
-        <v>Business Rates</v>
+        <v>Service Charge (Q3)</v>
       </c>
       <c r="C18">
-        <v>5000</v>
+        <v>12000</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>5000</v>
+        <v>12000</v>
       </c>
       <c r="F18" t="str">
         <v>No</v>
       </c>
       <c r="G18">
-        <v>286985</v>
+        <v>240791.2</v>
       </c>
       <c r="H18" t="str">
-        <v>Monthly payment</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>Jun 2026</v>
-      </c>
-      <c r="B19" t="str">
-        <v>Q3 Rent</v>
-      </c>
-      <c r="C19">
-        <v>32097</v>
-      </c>
-      <c r="D19">
-        <v>6419.4</v>
-      </c>
-      <c r="E19">
-        <v>38516.4</v>
-      </c>
-      <c r="F19" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="G19">
-        <v>248468.6</v>
-      </c>
-      <c r="H19" t="str">
-        <v>Quarter 3 rent payment</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>Jun 2026</v>
-      </c>
-      <c r="B20" t="str">
-        <v>Service Charge (Q3)</v>
-      </c>
-      <c r="C20">
-        <v>12000</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>12000</v>
-      </c>
-      <c r="F20" t="str">
-        <v>No</v>
-      </c>
-      <c r="G20">
-        <v>236468.6</v>
-      </c>
-      <c r="H20" t="str">
         <v>Quarterly service charge</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H20"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H18"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fix: Service charge £12k/year = £3k/quarter (not £12k/quarter)
</commit_message>
<xml_diff>
--- a/public/data/HOC_Investor_Dashboard_Template.xlsx
+++ b/public/data/HOC_Investor_Dashboard_Template.xlsx
@@ -580,16 +580,16 @@
         <v>Warehouse - Service Charge (Quarterly)</v>
       </c>
       <c r="B4">
+        <v>3000</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>12000</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>48000</v>
-      </c>
       <c r="E4" t="str">
-        <v>£12,000 per quarter - No VAT</v>
+        <v>£12,000 per year = £3,000 per quarter - No VAT</v>
       </c>
     </row>
     <row r="5">
@@ -1736,22 +1736,22 @@
         <v>Service Charge (Q1)</v>
       </c>
       <c r="C6">
-        <v>12000</v>
+        <v>3000</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>12000</v>
+        <v>3000</v>
       </c>
       <c r="F6" t="str">
         <v>No</v>
       </c>
       <c r="G6">
-        <v>407301.4</v>
+        <v>416301.4</v>
       </c>
       <c r="H6" t="str">
-        <v>Quarterly service charge - exempt</v>
+        <v>£12k/year = £3k/quarter</v>
       </c>
     </row>
     <row r="7">
@@ -1774,7 +1774,7 @@
         <v>No</v>
       </c>
       <c r="G7">
-        <v>402501.4</v>
+        <v>411501.4</v>
       </c>
       <c r="H7" t="str">
         <v>Annual insurance - exempt</v>
@@ -1800,7 +1800,7 @@
         <v>No</v>
       </c>
       <c r="G8">
-        <v>371824</v>
+        <v>406501.4</v>
       </c>
       <c r="H8" t="str">
         <v>Monthly - no VAT on rates</v>
@@ -1826,7 +1826,7 @@
         <v>No</v>
       </c>
       <c r="G9">
-        <v>366824</v>
+        <v>401501.4</v>
       </c>
       <c r="H9" t="str">
         <v>Monthly payment</v>
@@ -1852,7 +1852,7 @@
         <v>No</v>
       </c>
       <c r="G10">
-        <v>361824</v>
+        <v>396501.4</v>
       </c>
       <c r="H10" t="str">
         <v>Monthly payment</v>
@@ -1878,7 +1878,7 @@
         <v>No</v>
       </c>
       <c r="G11">
-        <v>356824</v>
+        <v>391501.4</v>
       </c>
       <c r="H11" t="str">
         <v>Monthly payment</v>
@@ -1904,7 +1904,7 @@
         <v>Yes</v>
       </c>
       <c r="G12">
-        <v>318307.6</v>
+        <v>352985</v>
       </c>
       <c r="H12" t="str">
         <v>Quarter 2 rent payment</v>
@@ -1918,22 +1918,22 @@
         <v>Service Charge (Q2)</v>
       </c>
       <c r="C13">
-        <v>12000</v>
+        <v>3000</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>12000</v>
+        <v>3000</v>
       </c>
       <c r="F13" t="str">
         <v>No</v>
       </c>
       <c r="G13">
-        <v>306307.6</v>
+        <v>349985</v>
       </c>
       <c r="H13" t="str">
-        <v>Quarterly service charge</v>
+        <v>£12k/year = £3k/quarter</v>
       </c>
     </row>
     <row r="14">
@@ -1956,7 +1956,7 @@
         <v>No</v>
       </c>
       <c r="G14">
-        <v>301307.6</v>
+        <v>344985</v>
       </c>
       <c r="H14" t="str">
         <v>Monthly payment</v>
@@ -1982,7 +1982,7 @@
         <v>No</v>
       </c>
       <c r="G15">
-        <v>296307.6</v>
+        <v>339985</v>
       </c>
       <c r="H15" t="str">
         <v>Monthly payment</v>
@@ -2008,7 +2008,7 @@
         <v>No</v>
       </c>
       <c r="G16">
-        <v>291307.6</v>
+        <v>334985</v>
       </c>
       <c r="H16" t="str">
         <v>Monthly payment</v>
@@ -2034,7 +2034,7 @@
         <v>Yes</v>
       </c>
       <c r="G17">
-        <v>252791.2</v>
+        <v>296468.6</v>
       </c>
       <c r="H17" t="str">
         <v>Quarter 3 rent payment</v>
@@ -2048,22 +2048,22 @@
         <v>Service Charge (Q3)</v>
       </c>
       <c r="C18">
-        <v>12000</v>
+        <v>3000</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>12000</v>
+        <v>3000</v>
       </c>
       <c r="F18" t="str">
         <v>No</v>
       </c>
       <c r="G18">
-        <v>240791.2</v>
+        <v>293468.6</v>
       </c>
       <c r="H18" t="str">
-        <v>Quarterly service charge</v>
+        <v>£12k/year = £3k/quarter</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Next major expense shows Dec total (£218,498.60), burn rate £19,239/month
</commit_message>
<xml_diff>
--- a/public/data/HOC_Investor_Dashboard_Template.xlsx
+++ b/public/data/HOC_Investor_Dashboard_Template.xlsx
@@ -464,10 +464,10 @@
         <v>Monthly Burn Rate</v>
       </c>
       <c r="B5">
-        <v>17000</v>
+        <v>19239</v>
       </c>
       <c r="C5" t="str">
-        <v>Estimated ongoing monthly costs after initial setup</v>
+        <v>Average monthly costs (rent, service charge, insurance, business rates)</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>Runway (Months)</v>
       </c>
       <c r="B6">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C6" t="str">
         <v>Calculated from remaining/burn rate</v>
@@ -486,7 +486,7 @@
         <v>Next Major Expense</v>
       </c>
       <c r="B7">
-        <v>245176</v>
+        <v>218498.6</v>
       </c>
       <c r="C7" t="str">
         <v>Due on landlord handover (Dec 19th)</v>
@@ -497,7 +497,7 @@
         <v>Next Expense Description</v>
       </c>
       <c r="B8" t="str">
-        <v>Warehouse Initial Payment</v>
+        <v>December 2025 Total</v>
       </c>
       <c r="C8" t="str">
         <v>Rent deposit, Q1 rent, service charge, insurance, business rates, legal</v>

</xml_diff>

<commit_message>
fix: Remove currency fluctuation and supplier lead times from risks
</commit_message>
<xml_diff>
--- a/public/data/HOC_Investor_Dashboard_Template.xlsx
+++ b/public/data/HOC_Investor_Dashboard_Template.xlsx
@@ -1355,7 +1355,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1463,22 +1463,22 @@
         <v>R003</v>
       </c>
       <c r="B4" t="str">
-        <v>Supplier Lead Times</v>
+        <v>Cash Flow Management</v>
       </c>
       <c r="C4" t="str">
-        <v>Amber</v>
+        <v>Green</v>
       </c>
       <c r="D4" t="str">
-        <v>Chinese New Year may impact initial stock delivery</v>
+        <v>Large initial payment due Dec 19th</v>
       </c>
       <c r="E4" t="str">
-        <v>Planning stock order ahead of CNY</v>
+        <v>Capital secured and available</v>
       </c>
       <c r="F4" t="str">
         <v>Open</v>
       </c>
       <c r="G4" t="str">
-        <v>Operations</v>
+        <v>Finance</v>
       </c>
       <c r="H4" t="str">
         <v>No</v>
@@ -1492,91 +1492,33 @@
         <v>R004</v>
       </c>
       <c r="B5" t="str">
-        <v>Currency Fluctuation</v>
+        <v>Staff Recruitment</v>
       </c>
       <c r="C5" t="str">
-        <v>Amber</v>
+        <v>Green</v>
       </c>
       <c r="D5" t="str">
-        <v>GBP/CNY exchange rate volatility</v>
+        <v>Need to hire warehouse and showroom staff</v>
       </c>
       <c r="E5" t="str">
-        <v>Building 5% currency buffer into pricing</v>
+        <v>Recruitment to begin Q1 2026</v>
       </c>
       <c r="F5" t="str">
         <v>Open</v>
       </c>
       <c r="G5" t="str">
-        <v>Finance</v>
+        <v>HR</v>
       </c>
       <c r="H5" t="str">
         <v>No</v>
       </c>
       <c r="I5" t="str">
-        <v>No</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>R005</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Cash Flow Management</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Green</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Large initial payment due Dec 19th</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Capital secured and available</v>
-      </c>
-      <c r="F6" t="str">
-        <v>Open</v>
-      </c>
-      <c r="G6" t="str">
-        <v>Finance</v>
-      </c>
-      <c r="H6" t="str">
-        <v>No</v>
-      </c>
-      <c r="I6" t="str">
-        <v>No</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>R006</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Staff Recruitment</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Green</v>
-      </c>
-      <c r="D7" t="str">
-        <v>Need to hire warehouse and showroom staff</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Recruitment to begin Q1 2026</v>
-      </c>
-      <c r="F7" t="str">
-        <v>Open</v>
-      </c>
-      <c r="G7" t="str">
-        <v>HR</v>
-      </c>
-      <c r="H7" t="str">
-        <v>No</v>
-      </c>
-      <c r="I7" t="str">
         <v>No</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I5"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fix: Correct rent structure - deposit at full rate, 2026 at 50% rate
RENT STRUCTURE:
- 2026 (50% reduced): £10,699/month + VAT = £12,838.80
- 2027+ (full rate): £21,398/month + VAT = £25,677.60
- 7 month deposit (based on full rate): £149,786 + VAT = £179,743.20

December 2025 total: £244,176.20
Closing balance Jun 2026: £267,791
</commit_message>
<xml_diff>
--- a/public/data/HOC_Investor_Dashboard_Template.xlsx
+++ b/public/data/HOC_Investor_Dashboard_Template.xlsx
@@ -486,7 +486,7 @@
         <v>Next Major Expense</v>
       </c>
       <c r="B7">
-        <v>218498.6</v>
+        <v>244176.2</v>
       </c>
       <c r="C7" t="str">
         <v>Due on landlord handover (Dec 19th)</v>
@@ -500,7 +500,7 @@
         <v>December 2025 Total</v>
       </c>
       <c r="C8" t="str">
-        <v>Rent deposit, Q1 rent, service charge, insurance, business rates, legal</v>
+        <v>Rent deposit (7mo @ full rate), Q1 rent (50% rate), service charge, insurance, business rates, legal</v>
       </c>
     </row>
   </sheetData>
@@ -543,24 +543,24 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Warehouse - Rent Deposit (7 months)</v>
+        <v>Warehouse - Rent Deposit (7 months @ full rate)</v>
       </c>
       <c r="B2">
-        <v>154065.6</v>
+        <v>179743.2</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>154065.6</v>
+        <v>179743.2</v>
       </c>
       <c r="E2" t="str">
-        <v>£128,388 + VAT (£25,677.60) - Due Dec 19th</v>
+        <v>£149,786 + VAT (£29,957.20) - Based on full rate £21,398/mo</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Warehouse - Q1 Rent</v>
+        <v>Warehouse - Q1 Rent (50% reduced rate)</v>
       </c>
       <c r="B3">
         <v>38516.4</v>
@@ -572,7 +572,7 @@
         <v>38516.4</v>
       </c>
       <c r="E3" t="str">
-        <v>£32,097 + VAT (£6,419.40) - Due Dec 19th</v>
+        <v>£32,097 + VAT (£6,419.40) - 2026 rate: £10,699/mo</v>
       </c>
     </row>
     <row r="4">
@@ -1623,25 +1623,25 @@
         <v>Dec 2025</v>
       </c>
       <c r="B4" t="str">
-        <v>Rent Deposit (7 months)</v>
+        <v>Rent Deposit (7mo @ full rate)</v>
       </c>
       <c r="C4">
-        <v>128388</v>
+        <v>149786</v>
       </c>
       <c r="D4">
-        <v>25677.6</v>
+        <v>29957.2</v>
       </c>
       <c r="E4">
-        <v>154065.6</v>
+        <v>179743.2</v>
       </c>
       <c r="F4" t="str">
         <v>Yes</v>
       </c>
       <c r="G4">
-        <v>457817.8</v>
+        <v>432140.2</v>
       </c>
       <c r="H4" t="str">
-        <v>7 months deposit</v>
+        <v>7 months @ £21,398/mo (2027 rate)</v>
       </c>
     </row>
     <row r="5">
@@ -1649,7 +1649,7 @@
         <v>Dec 2025</v>
       </c>
       <c r="B5" t="str">
-        <v>Q1 Rent</v>
+        <v>Q1 Rent (50% reduced)</v>
       </c>
       <c r="C5">
         <v>32097</v>
@@ -1664,10 +1664,10 @@
         <v>Yes</v>
       </c>
       <c r="G5">
-        <v>419301.4</v>
+        <v>393623.8</v>
       </c>
       <c r="H5" t="str">
-        <v>Quarter 1 rent payment</v>
+        <v>2026 rate: £10,699/mo</v>
       </c>
     </row>
     <row r="6">
@@ -1690,7 +1690,7 @@
         <v>No</v>
       </c>
       <c r="G6">
-        <v>416301.4</v>
+        <v>390623.8</v>
       </c>
       <c r="H6" t="str">
         <v>£12k/year = £3k/quarter</v>
@@ -1716,7 +1716,7 @@
         <v>No</v>
       </c>
       <c r="G7">
-        <v>411501.4</v>
+        <v>385823.8</v>
       </c>
       <c r="H7" t="str">
         <v>Annual insurance - exempt</v>
@@ -1742,7 +1742,7 @@
         <v>No</v>
       </c>
       <c r="G8">
-        <v>406501.4</v>
+        <v>380823.8</v>
       </c>
       <c r="H8" t="str">
         <v>Monthly - no VAT on rates</v>
@@ -1768,7 +1768,7 @@
         <v>No</v>
       </c>
       <c r="G9">
-        <v>401501.4</v>
+        <v>375823.8</v>
       </c>
       <c r="H9" t="str">
         <v>Monthly payment</v>
@@ -1794,7 +1794,7 @@
         <v>No</v>
       </c>
       <c r="G10">
-        <v>396501.4</v>
+        <v>370823.8</v>
       </c>
       <c r="H10" t="str">
         <v>Monthly payment</v>
@@ -1820,7 +1820,7 @@
         <v>No</v>
       </c>
       <c r="G11">
-        <v>391501.4</v>
+        <v>365823.8</v>
       </c>
       <c r="H11" t="str">
         <v>Monthly payment</v>
@@ -1831,7 +1831,7 @@
         <v>Mar 2026</v>
       </c>
       <c r="B12" t="str">
-        <v>Q2 Rent</v>
+        <v>Q2 Rent (50% reduced)</v>
       </c>
       <c r="C12">
         <v>32097</v>
@@ -1846,10 +1846,10 @@
         <v>Yes</v>
       </c>
       <c r="G12">
-        <v>352985</v>
+        <v>327307.4</v>
       </c>
       <c r="H12" t="str">
-        <v>Quarter 2 rent payment</v>
+        <v>2026 rate: £10,699/mo</v>
       </c>
     </row>
     <row r="13">
@@ -1872,7 +1872,7 @@
         <v>No</v>
       </c>
       <c r="G13">
-        <v>349985</v>
+        <v>324307.4</v>
       </c>
       <c r="H13" t="str">
         <v>£12k/year = £3k/quarter</v>
@@ -1898,7 +1898,7 @@
         <v>No</v>
       </c>
       <c r="G14">
-        <v>344985</v>
+        <v>319307.4</v>
       </c>
       <c r="H14" t="str">
         <v>Monthly payment</v>
@@ -1924,7 +1924,7 @@
         <v>No</v>
       </c>
       <c r="G15">
-        <v>339985</v>
+        <v>314307.4</v>
       </c>
       <c r="H15" t="str">
         <v>Monthly payment</v>
@@ -1950,7 +1950,7 @@
         <v>No</v>
       </c>
       <c r="G16">
-        <v>334985</v>
+        <v>309307.4</v>
       </c>
       <c r="H16" t="str">
         <v>Monthly payment</v>
@@ -1961,7 +1961,7 @@
         <v>Jun 2026</v>
       </c>
       <c r="B17" t="str">
-        <v>Q3 Rent</v>
+        <v>Q3 Rent (50% reduced)</v>
       </c>
       <c r="C17">
         <v>32097</v>
@@ -1976,10 +1976,10 @@
         <v>Yes</v>
       </c>
       <c r="G17">
-        <v>296468.6</v>
+        <v>270791</v>
       </c>
       <c r="H17" t="str">
-        <v>Quarter 3 rent payment</v>
+        <v>2026 rate: £10,699/mo</v>
       </c>
     </row>
     <row r="18">
@@ -2002,7 +2002,7 @@
         <v>No</v>
       </c>
       <c r="G18">
-        <v>293468.6</v>
+        <v>267791</v>
       </c>
       <c r="H18" t="str">
         <v>£12k/year = £3k/quarter</v>

</xml_diff>

<commit_message>
fix: Accurate runway (17 months) with 2026/2027 burn rates
2026 burn (reduced rent): £19,239/month
2027+ burn (full rent): £32,078/month
Runway: ~17 months (until May 2027)
</commit_message>
<xml_diff>
--- a/public/data/HOC_Investor_Dashboard_Template.xlsx
+++ b/public/data/HOC_Investor_Dashboard_Template.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -461,51 +461,62 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Monthly Burn Rate</v>
+        <v>Monthly Burn Rate (2026)</v>
       </c>
       <c r="B5">
         <v>19239</v>
       </c>
       <c r="C5" t="str">
-        <v>Average monthly costs (rent, service charge, insurance, business rates)</v>
+        <v>2026 average (50% reduced rent): £5k rates + £12.8k rent + £1k service + £0.4k insurance</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Runway (Months)</v>
+        <v>Monthly Burn Rate (2027+)</v>
       </c>
       <c r="B6">
-        <v>32</v>
+        <v>32078</v>
       </c>
       <c r="C6" t="str">
-        <v>Calculated from remaining/burn rate</v>
+        <v>2027+ average (full rent): £5k rates + £25.7k rent + £1k service + £0.4k insurance</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Next Major Expense</v>
+        <v>Runway (Months)</v>
       </c>
       <c r="B7">
-        <v>244176.2</v>
+        <v>17</v>
       </c>
       <c r="C7" t="str">
-        <v>Due on landlord handover (Dec 19th)</v>
+        <v>Until ~May 2027 (12 months 2026 + ~5 months 2027)</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
+        <v>Next Major Expense</v>
+      </c>
+      <c r="B8">
+        <v>244176.2</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Due on landlord handover (Dec 19th)</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
         <v>Next Expense Description</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B9" t="str">
         <v>December 2025 Total</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C9" t="str">
         <v>Rent deposit (7mo @ full rate), Q1 rent (50% rate), service charge, insurance, business rates, legal</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C9"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>